<commit_message>
edit details and reservation test cases
</commit_message>
<xml_diff>
--- a/Car_TestCases/Car_Details_and_Reservation.xlsx
+++ b/Car_TestCases/Car_Details_and_Reservation.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Test case ID</t>
   </si>
@@ -58,27 +58,61 @@
     <t>Car_Details_01</t>
   </si>
   <si>
-    <t>Car_SRS_45</t>
-  </si>
-  <si>
-    <t>Validate that "MYPROFILE" button is exist in the header</t>
-  </si>
-  <si>
-    <t>1) open URL "http://CarPurchasing"
-2)Login with exist account</t>
-  </si>
-  <si>
-    <t>User name: customer
-password: soso.soso123</t>
-  </si>
-  <si>
-    <t>UI</t>
-  </si>
-  <si>
-    <t>MYPROFILE button Should displayed in top right of the page.</t>
-  </si>
-  <si>
     <t>Fatma</t>
+  </si>
+  <si>
+    <t>Car_Details_02</t>
+  </si>
+  <si>
+    <t>Car_Details_03</t>
+  </si>
+  <si>
+    <t>Car_Details_04</t>
+  </si>
+  <si>
+    <t>Car_Details_05</t>
+  </si>
+  <si>
+    <t>Car_Details_06</t>
+  </si>
+  <si>
+    <t>Car_Details_07</t>
+  </si>
+  <si>
+    <t>Car_Details_08</t>
+  </si>
+  <si>
+    <t>Car_Details_09</t>
+  </si>
+  <si>
+    <t>Car_Details_10</t>
+  </si>
+  <si>
+    <t>Car_Details_11</t>
+  </si>
+  <si>
+    <t>Car_Details_12</t>
+  </si>
+  <si>
+    <t>Car_Details_13</t>
+  </si>
+  <si>
+    <t>Car_Details_14</t>
+  </si>
+  <si>
+    <t>Car_Details_15</t>
+  </si>
+  <si>
+    <t>Car_Details_16</t>
+  </si>
+  <si>
+    <t>Car_Details_17</t>
+  </si>
+  <si>
+    <t>Car_Details_18</t>
+  </si>
+  <si>
+    <t>Car_Details_19</t>
   </si>
 </sst>
 </file>
@@ -160,55 +194,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>50417</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>3038448</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>2000250</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="16795367" y="400050"/>
-          <a:ext cx="2988031" cy="1885950"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -498,10 +483,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:M20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.85546875" defaultRowHeight="89.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -563,30 +548,102 @@
       <c r="A2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="3"/>
+      <c r="J2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="2" t="s">
+    </row>
+    <row r="3" spans="1:13" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" s="2" t="s">
+    </row>
+    <row r="7" spans="1:13" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="2" t="s">
+    </row>
+    <row r="8" spans="1:13" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update Car details and reservation test cases
</commit_message>
<xml_diff>
--- a/Car_TestCases/Car_Details_and_Reservation.xlsx
+++ b/Car_TestCases/Car_Details_and_Reservation.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Test case ID</t>
   </si>
@@ -113,6 +113,9 @@
   </si>
   <si>
     <t>Car_Details_19</t>
+  </si>
+  <si>
+    <t>Car_SRS_20</t>
   </si>
 </sst>
 </file>
@@ -173,11 +176,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -485,8 +488,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:I2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.85546875" defaultRowHeight="89.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -503,7 +506,7 @@
     <col min="10" max="16384" width="20.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="4" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="3" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -548,7 +551,9 @@
       <c r="A2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="3"/>
+      <c r="B2" s="4" t="s">
+        <v>33</v>
+      </c>
       <c r="J2" s="2" t="s">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
Update car details and reservation (add test case for guest )
</commit_message>
<xml_diff>
--- a/Car_TestCases/Car_Details_and_Reservation.xlsx
+++ b/Car_TestCases/Car_Details_and_Reservation.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="51">
   <si>
     <t>Test case ID</t>
   </si>
@@ -82,9 +82,6 @@
   </si>
   <si>
     <t>passed</t>
-  </si>
-  <si>
-    <t>Validate "See more" button functionality</t>
   </si>
   <si>
     <t>Validate UI of car details page</t>
@@ -164,6 +161,25 @@
   </si>
   <si>
     <t>jannat</t>
+  </si>
+  <si>
+    <t>Car_Details_03</t>
+  </si>
+  <si>
+    <t>Car_SRS_07</t>
+  </si>
+  <si>
+    <t>1) open URL "http://CarPurchasing"
+2)don't login</t>
+  </si>
+  <si>
+    <t>Guest should be redirected to a registration  page</t>
+  </si>
+  <si>
+    <t>Validate "See more" button functionality for a guest</t>
+  </si>
+  <si>
+    <t>Validate "See more" button functionality for a user</t>
   </si>
 </sst>
 </file>
@@ -276,13 +292,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>2</xdr:row>
+      <xdr:row>3</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>3019425</xdr:colOff>
-      <xdr:row>2</xdr:row>
+      <xdr:row>3</xdr:row>
       <xdr:rowOff>1628775</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -318,13 +334,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>3000375</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>1600200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -646,10 +662,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M7"/>
+  <dimension ref="A1:M8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.85546875" defaultRowHeight="131.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -718,7 +734,7 @@
         <v>17</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>19</v>
@@ -727,16 +743,19 @@
         <v>18</v>
       </c>
       <c r="G2" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>40</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>41</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>14</v>
       </c>
       <c r="K2" s="4" t="s">
         <v>21</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="131.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -744,25 +763,22 @@
         <v>15</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>23</v>
+        <v>49</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>18</v>
+        <v>47</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="J3" s="4" t="s">
         <v>14</v>
@@ -771,80 +787,80 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:13" s="5" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7"/>
+    <row r="4" spans="1:13" ht="131.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>44</v>
+      </c>
     </row>
-    <row r="5" spans="1:13" ht="131.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="1:13" s="5" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="K5" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="L5" s="4" t="s">
-        <v>45</v>
-      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
     </row>
     <row r="6" spans="1:13" ht="131.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>17</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>19</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="J6" s="4" t="s">
         <v>14</v>
@@ -852,31 +868,31 @@
       <c r="K6" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="L6" s="4" t="s">
-        <v>45</v>
+      <c r="M6" s="4" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="131.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B7" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>31</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>36</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>19</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H7" s="4" t="s">
         <v>38</v>
@@ -887,13 +903,48 @@
       <c r="K7" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="L7" s="4" t="s">
-        <v>45</v>
+      <c r="M7" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="131.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M8" s="4" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
add test case Car_Reservation_04
</commit_message>
<xml_diff>
--- a/Car_TestCases/Car_Details_and_Reservation.xlsx
+++ b/Car_TestCases/Car_Details_and_Reservation.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="55">
   <si>
     <t>Test case ID</t>
   </si>
@@ -180,6 +180,22 @@
   </si>
   <si>
     <t>Validate "See more" button functionality for a user</t>
+  </si>
+  <si>
+    <t>Car_Reservation_04</t>
+  </si>
+  <si>
+    <t>Check if the date of reservation is correct after reserve a car</t>
+  </si>
+  <si>
+    <t>User should be redirected to Reserved cars page
+and this page contains all the cars reserved by the user before which written on it reserved by username</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1)From the home page click on "see more" button at any car
+2)Click on Reserve button 
+3)From the header click on "Reserved cars" 
+4)check if the car exists and the data is right on it </t>
   </si>
 </sst>
 </file>
@@ -662,10 +678,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M8"/>
+  <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+    <sheetView tabSelected="1" topLeftCell="F8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.85546875" defaultRowHeight="131.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -942,6 +958,41 @@
         <v>44</v>
       </c>
     </row>
+    <row r="9" spans="1:13" ht="131.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K9" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M9" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A5:K5"/>

</xml_diff>